<commit_message>
Code clean-up and added variable Known Consignor ref
</commit_message>
<xml_diff>
--- a/Data/SdfTemplate.xlsx
+++ b/Data/SdfTemplate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wau0195\source\repos\Security Declaration Form Generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wau0195\source\repos\Security-Declaration-Form-Generator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8D4C8D-7150-4325-9881-951FDCD5B8BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4580B619-1820-4BAE-83C2-400F74159C53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{17262DEC-3080-492C-8D6A-12E833501BD0}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <definedName name="Consignor">Declaration!$B$11</definedName>
     <definedName name="Contents_Of_Consignment">Declaration!$B$15</definedName>
     <definedName name="Issue_Date">Declaration!$B$19</definedName>
+    <definedName name="Known_Consignor_Ref">Declaration!$A$13</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Declaration!$A$1:$B$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -485,7 +486,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97AF746B-6B7B-4231-A2F8-98E84967D9E6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -823,7 +824,7 @@
   <dimension ref="A1:XFC1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B8"/>
+      <selection activeCell="A13" sqref="A13:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="27" zeroHeight="1" x14ac:dyDescent="0.35"/>
@@ -1112,27 +1113,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1041" r:id="rId4" name="lblCurrentFullName">
-          <controlPr defaultSize="0" print="0" autoLine="0" autoPict="0" r:id="rId5">
+        <control shapeId="1034" r:id="rId4" name="lblSelectedPaperPrinter">
+          <controlPr defaultSize="0" print="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>1628775</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>3943350</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>3914775</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>295275</xdr:rowOff>
+                <xdr:colOff>3714750</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1041" r:id="rId4" name="lblCurrentFullName"/>
+        <control shapeId="1034" r:id="rId4" name="lblSelectedPaperPrinter"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -1162,27 +1163,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1034" r:id="rId8" name="lblSelectedPaperPrinter">
-          <controlPr defaultSize="0" print="0" autoLine="0" r:id="rId9">
+        <control shapeId="1041" r:id="rId8" name="lblCurrentFullName">
+          <controlPr defaultSize="0" print="0" autoLine="0" autoPict="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>3943350</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>1628775</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>3714750</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>266700</xdr:rowOff>
+                <xdr:colOff>3914775</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>295275</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1034" r:id="rId8" name="lblSelectedPaperPrinter"/>
+        <control shapeId="1041" r:id="rId8" name="lblCurrentFullName"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Fixed issue with date formatting.
</commit_message>
<xml_diff>
--- a/Data/SdfTemplate.xlsx
+++ b/Data/SdfTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wau0195\source\repos\Security-Declaration-Form-Generator\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wau0195\source\repos\Weidmueller\Security-Declaration-Form-Generator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4580B619-1820-4BAE-83C2-400F74159C53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BC0D23-1232-47A2-9824-EF5776C8864F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{17262DEC-3080-492C-8D6A-12E833501BD0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{17262DEC-3080-492C-8D6A-12E833501BD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Declaration" sheetId="1" r:id="rId1"/>
@@ -93,6 +93,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy\ hh:mm"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -242,9 +245,6 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -261,6 +261,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -823,8 +826,8 @@
   </sheetPr>
   <dimension ref="A1:XFC1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:B13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="27" zeroHeight="1" x14ac:dyDescent="0.35"/>
@@ -853,10 +856,10 @@
       <c r="B3" s="6"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="22"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="3"/>
       <c r="E4" s="7"/>
     </row>
@@ -873,10 +876,10 @@
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="23"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -885,10 +888,10 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="22"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="4"/>
@@ -897,10 +900,10 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="23"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="4"/>
@@ -929,10 +932,10 @@
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="20"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -949,10 +952,10 @@
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="25"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
@@ -964,7 +967,7 @@
       <c r="A15" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="21"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -990,7 +993,7 @@
       <c r="A19" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="18"/>
+      <c r="B19" s="25"/>
       <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:6" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1000,13 +1003,13 @@
       <c r="A21" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="19"/>
+      <c r="B21" s="18"/>
     </row>
     <row r="22" spans="1:6" s="1" customFormat="1" ht="159.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="24"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
Major changes in line with Dept Home Affairs Regulations
</commit_message>
<xml_diff>
--- a/Data/SdfTemplate.xlsx
+++ b/Data/SdfTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wau0195\source\repos\Weidmueller\Security-Declaration-Form-Generator\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wau0195\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BC0D23-1232-47A2-9824-EF5776C8864F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD327554-D815-4C5C-81D7-CEF315DDAAD1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{17262DEC-3080-492C-8D6A-12E833501BD0}"/>
   </bookViews>
@@ -16,11 +16,13 @@
     <sheet name="Declaration" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="Cargo_Dest_Address">Declaration!$B$8</definedName>
+    <definedName name="Cargo_Dest_Name">Declaration!$B$6</definedName>
     <definedName name="Consignment_Number">Declaration!$B$17</definedName>
-    <definedName name="Consignor">Declaration!$B$11</definedName>
+    <definedName name="Consignor">Declaration!$B$13</definedName>
     <definedName name="Contents_Of_Consignment">Declaration!$B$15</definedName>
     <definedName name="Issue_Date">Declaration!$B$19</definedName>
-    <definedName name="Known_Consignor_Ref">Declaration!$A$13</definedName>
+    <definedName name="Known_Consignor_Ref">Declaration!$B$11</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Declaration!$A$1:$B$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -41,38 +43,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>WEIDMULLER PTY LTD</t>
   </si>
   <si>
-    <t>CONSIGNMENT SECURITY DECLARATION</t>
-  </si>
-  <si>
-    <t>43 Huntingwood Drive</t>
-  </si>
-  <si>
-    <t>Huntingwood  NSW.  2148</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Security Status Issued by: </t>
-  </si>
-  <si>
     <t>Signature:</t>
   </si>
   <si>
-    <t>Security Status Issued on:</t>
-  </si>
-  <si>
-    <t>KNOWN CONSIGNOR: AU-KC/01327-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contents of consignment: </t>
-  </si>
-  <si>
-    <t>Origin:</t>
-  </si>
-  <si>
     <t>Ph: +61 (0) 2 9671 9999</t>
   </si>
   <si>
@@ -82,11 +60,89 @@
     <t>Airport or ICAO code to which the cargo is being transported:</t>
   </si>
   <si>
-    <t>The RACA operator will kindly complete the 'Airport or ICAO code to which the cargo is being transported' section.
-This declaration confirms the cargo is not required to be examined as our cargo has received clearance in accordance with ATSR 4.41C</t>
-  </si>
-  <si>
     <t/>
+  </si>
+  <si>
+    <t>Cargo Origin Address:</t>
+  </si>
+  <si>
+    <t>43 Huntingwood Drive, Huntingwood</t>
+  </si>
+  <si>
+    <t>NSW  2148  Australia</t>
+  </si>
+  <si>
+    <t>Cargo Destination Address:</t>
+  </si>
+  <si>
+    <t>Security Declaration Issued on:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="22"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Clearance Statement:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Cargo is not required to be examined to receive clearance as it has been originated from a Known Consignor and been handled in accordance with r4.42D(c) of the Aviation Transport Security Regulations 2015 and the Known Consignor’s approved security program. </t>
+    </r>
+  </si>
+  <si>
+    <t>Security Declaration Issued by:</t>
+  </si>
+  <si>
+    <t>Contents of Consignment:</t>
+  </si>
+  <si>
+    <t>The RACA operator will kindly complete the "Airport or ICAO code to which the cargo is being transported" section.</t>
+  </si>
+  <si>
+    <t>SECURITY DECLARATION</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Status:  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>KNOWN CONSIGNOR  &gt;&gt;&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -94,9 +150,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy\ hh:mm"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -152,6 +208,34 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -167,7 +251,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -204,11 +288,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -220,50 +355,93 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -512,7 +690,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6057900" y="266700"/>
-          <a:ext cx="2390775" cy="323850"/>
+          <a:ext cx="2390775" cy="321252"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -826,8 +1004,8 @@
   </sheetPr>
   <dimension ref="A1:XFC1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="27" zeroHeight="1" x14ac:dyDescent="0.35"/>
@@ -851,23 +1029,25 @@
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="21"/>
+    <row r="3" spans="1:8" s="1" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="35"/>
+    </row>
+    <row r="4" spans="1:8" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="3"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:8" s="1" customFormat="1" ht="27.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="16"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -875,11 +1055,11 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="22" t="s">
+    <row r="6" spans="1:8" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="22"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -887,11 +1067,11 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="22"/>
+    <row r="7" spans="1:8" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="39"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="4"/>
@@ -899,11 +1079,11 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="22"/>
+    <row r="8" spans="1:8" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="33"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="4"/>
@@ -911,11 +1091,11 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="10"/>
+    <row r="9" spans="1:8" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="33"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="4"/>
@@ -923,7 +1103,9 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="41"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -931,11 +1113,11 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="19"/>
+    <row r="11" spans="1:8" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="26"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -943,7 +1125,9 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="25"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -951,78 +1135,82 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="24" t="s">
-        <v>7</v>
+    <row r="13" spans="1:8" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="16" t="s">
+        <v>12</v>
       </c>
       <c r="B13" s="24"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:8" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
+    <row r="14" spans="1:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="17"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="20"/>
+    <row r="15" spans="1:8" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="28"/>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
+    <row r="16" spans="1:8" s="1" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="17"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:6" s="1" customFormat="1" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="17" t="s">
+      <c r="A17" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="19"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" s="1" customFormat="1" ht="27.75" x14ac:dyDescent="0.35">
+      <c r="A19" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" ht="69.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="12"/>
+    </row>
+    <row r="22" spans="1:6" s="1" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" s="1" customFormat="1" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="A19" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" ht="69.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="18"/>
-    </row>
-    <row r="22" spans="1:6" s="1" customFormat="1" ht="159.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="23"/>
+      <c r="B22" s="38"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
+    <row r="23" spans="1:6" s="1" customFormat="1" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="14"/>
       <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:6" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="15" t="s">
-        <v>5</v>
+      <c r="A24" s="10" t="s">
+        <v>1</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="3"/>
@@ -1102,41 +1290,41 @@
     <row r="1048576" ht="137.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B6:B7"/>
     <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A3:B4"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="74" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1034" r:id="rId4" name="lblSelectedPaperPrinter">
-          <controlPr defaultSize="0" print="0" autoLine="0" r:id="rId5">
+        <control shapeId="1041" r:id="rId4" name="lblCurrentFullName">
+          <controlPr defaultSize="0" print="0" autoLine="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>3943350</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>1628775</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>3714750</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>266700</xdr:rowOff>
+                <xdr:colOff>3914775</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>304800</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1034" r:id="rId4" name="lblSelectedPaperPrinter"/>
+        <control shapeId="1041" r:id="rId4" name="lblCurrentFullName"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -1166,27 +1354,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1041" r:id="rId8" name="lblCurrentFullName">
-          <controlPr defaultSize="0" print="0" autoLine="0" autoPict="0" r:id="rId9">
+        <control shapeId="1034" r:id="rId8" name="lblSelectedPaperPrinter">
+          <controlPr defaultSize="0" print="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>1628775</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>3943350</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>3914775</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>295275</xdr:rowOff>
+                <xdr:colOff>3714750</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1041" r:id="rId8" name="lblCurrentFullName"/>
+        <control shapeId="1034" r:id="rId8" name="lblSelectedPaperPrinter"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Added Cargo Destination, changed Toll prefix value, redesigned layout of Main form, redsigned layout of SdfTemplate.xlsx
</commit_message>
<xml_diff>
--- a/Data/SdfTemplate.xlsx
+++ b/Data/SdfTemplate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wau0195\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wau0195\source\repos\Security-Declaration-Form-Generator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD327554-D815-4C5C-81D7-CEF315DDAAD1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F51D4B-A3A8-4F85-B527-E873CD7F4395}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{17262DEC-3080-492C-8D6A-12E833501BD0}"/>
   </bookViews>
@@ -368,9 +368,6 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -402,6 +399,19 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -410,39 +420,29 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -604,7 +604,7 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>3914775</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>295275</xdr:rowOff>
+          <xdr:rowOff>304800</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1004,8 +1004,8 @@
   </sheetPr>
   <dimension ref="A1:XFC1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="27" zeroHeight="1" x14ac:dyDescent="0.35"/>
@@ -1030,22 +1030,22 @@
       <c r="B2" s="6"/>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="35"/>
+      <c r="B3" s="39"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="3"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" ht="27.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="3"/>
@@ -1056,10 +1056,10 @@
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="39"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -1068,10 +1068,10 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="39"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="4"/>
@@ -1080,10 +1080,10 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="33"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="4"/>
@@ -1092,10 +1092,10 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="33"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="4"/>
@@ -1104,8 +1104,8 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="41"/>
-      <c r="B10" s="34"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -1114,10 +1114,10 @@
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="26"/>
+      <c r="B11" s="25"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1126,8 +1126,8 @@
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="25"/>
-      <c r="B12" s="27"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="26"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -1136,27 +1136,27 @@
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="24"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:8" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="28"/>
+      <c r="B15" s="32"/>
       <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:8" s="1" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="17"/>
-      <c r="B16" s="29"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:6" s="1" customFormat="1" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1169,24 +1169,24 @@
       <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:6" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="19"/>
-      <c r="B18" s="20"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="19"/>
       <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:6" s="1" customFormat="1" ht="27.75" x14ac:dyDescent="0.35">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="20" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="13"/>
       <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:6" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
       <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:6" ht="69.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="22" t="s">
         <v>4</v>
       </c>
       <c r="B21" s="12"/>
@@ -1201,14 +1201,14 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" s="1" customFormat="1" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="s">
+    <row r="23" spans="1:6" s="1" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="14"/>
+      <c r="B23" s="41"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:6" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" s="1" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
         <v>1</v>
       </c>
@@ -1290,12 +1290,12 @@
     <row r="1048576" ht="137.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A3:B4"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A3:B4"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -1304,27 +1304,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1041" r:id="rId4" name="lblCurrentFullName">
-          <controlPr defaultSize="0" print="0" autoLine="0" autoPict="0" r:id="rId5">
+        <control shapeId="1034" r:id="rId4" name="lblSelectedPaperPrinter">
+          <controlPr defaultSize="0" print="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>1628775</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>3943350</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>3914775</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>304800</xdr:rowOff>
+                <xdr:colOff>3714750</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1041" r:id="rId4" name="lblCurrentFullName"/>
+        <control shapeId="1034" r:id="rId4" name="lblSelectedPaperPrinter"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -1354,27 +1354,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1034" r:id="rId8" name="lblSelectedPaperPrinter">
-          <controlPr defaultSize="0" print="0" autoLine="0" r:id="rId9">
+        <control shapeId="1041" r:id="rId8" name="lblCurrentFullName">
+          <controlPr defaultSize="0" print="0" autoLine="0" autoPict="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>3943350</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>1628775</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>3714750</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>266700</xdr:rowOff>
+                <xdr:colOff>3914775</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>304800</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1034" r:id="rId8" name="lblSelectedPaperPrinter"/>
+        <control shapeId="1041" r:id="rId8" name="lblCurrentFullName"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>